<commit_message>
add data for web
</commit_message>
<xml_diff>
--- a/data/han/수질/대성리_2015.xlsx
+++ b/data/han/수질/대성리_2015.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotech/Desktop/NIA/water quality/DATA/data/han/수질/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD546AE7-D158-2C4B-A567-2162354472D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
   <si>
     <t>dt</t>
   </si>
@@ -221,51 +229,27 @@
     <t>20150106</t>
   </si>
   <si>
-    <t>2015-02-30 12:00</t>
-  </si>
-  <si>
     <t>20150202</t>
   </si>
   <si>
-    <t>2015-03-45 12:00</t>
-  </si>
-  <si>
     <t>20150316</t>
   </si>
   <si>
-    <t>2015-04-60 12:00</t>
-  </si>
-  <si>
     <t>20150406</t>
   </si>
   <si>
-    <t>2015-05-75 12:00</t>
-  </si>
-  <si>
     <t>20150504</t>
   </si>
   <si>
-    <t>2015-06-90 12:00</t>
-  </si>
-  <si>
     <t>20150601</t>
   </si>
   <si>
-    <t>2015-07-10 12:00</t>
-  </si>
-  <si>
     <t>20150706</t>
   </si>
   <si>
-    <t>2015-08-12 12:00</t>
-  </si>
-  <si>
     <t>20150803</t>
   </si>
   <si>
-    <t>2015-09-13 12:00</t>
-  </si>
-  <si>
     <t>20150907</t>
   </si>
   <si>
@@ -275,13 +259,7 @@
     <t>20151005</t>
   </si>
   <si>
-    <t>2015-11-16 12:00</t>
-  </si>
-  <si>
     <t>20151102</t>
-  </si>
-  <si>
-    <t>2015-12-18 12:00</t>
   </si>
   <si>
     <t>20151207</t>
@@ -290,25 +268,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="178" formatCode="0.0000"/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -326,25 +313,40 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,10 +355,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -602,83 +604,81 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:BJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="17.44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.78" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.67" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.78" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.78" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.78" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.44" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.89" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.78" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.22" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.44" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.44" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.44" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.11" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.67" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.78" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.44" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.67" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.56" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.78" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.22" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.22" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="8" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:62">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +866,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:62">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -895,9 +895,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>69</v>
+    <row r="3" spans="1:62">
+      <c r="A3" s="7">
+        <v>42050.5</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -921,12 +921,12 @@
         <v>67</v>
       </c>
       <c r="AB3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>71</v>
+    <row r="4" spans="1:62">
+      <c r="A4" s="7">
+        <v>42078.5</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
@@ -950,10 +950,10 @@
         <v>67</v>
       </c>
       <c r="AB4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AC4" s="3">
-        <v>0.095000000000000001</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="AD4" s="4">
         <v>1.4371</v>
@@ -962,13 +962,13 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="AF4" s="5">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="AG4">
         <v>106</v>
       </c>
       <c r="AH4" s="5">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="AI4" s="5">
         <v>1.2</v>
@@ -980,30 +980,30 @@
         <v>1.9590000000000001</v>
       </c>
       <c r="AL4" s="3">
-        <v>0.0070000000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AN4" s="5">
         <v>4.5999999999999996</v>
       </c>
       <c r="AO4" s="5">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AP4" s="3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AQ4" s="3">
         <v>1.9510000000000001</v>
       </c>
       <c r="AR4" s="3">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AS4" s="5">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>73</v>
+    <row r="5" spans="1:62">
+      <c r="A5" s="7">
+        <v>42109.5</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -1027,7 +1027,7 @@
         <v>67</v>
       </c>
       <c r="AB5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AC5" s="3">
         <v>0.14299999999999999</v>
@@ -1036,10 +1036,10 @@
         <v>1.4650000000000001</v>
       </c>
       <c r="AE5" s="5">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF5" s="5">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="AG5">
         <v>111</v>
@@ -1057,30 +1057,30 @@
         <v>2.262</v>
       </c>
       <c r="AL5" s="3">
-        <v>0.014999999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AN5" s="5">
-        <v>10.300000000000001</v>
+        <v>10.3</v>
       </c>
       <c r="AO5" s="5">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="AP5" s="3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AQ5" s="5">
         <v>2.2000000000000002</v>
       </c>
       <c r="AR5" s="3">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AS5" s="5">
         <v>1.8</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>75</v>
+    <row r="6" spans="1:62">
+      <c r="A6" s="7">
+        <v>42139.5</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
@@ -1104,10 +1104,10 @@
         <v>67</v>
       </c>
       <c r="AB6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AC6" s="3">
-        <v>0.036999999999999998</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="AD6" s="4">
         <v>1.5916999999999999</v>
@@ -1122,7 +1122,7 @@
         <v>115</v>
       </c>
       <c r="AH6" s="5">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="AI6" s="5">
         <v>1.8</v>
@@ -1131,33 +1131,33 @@
         <v>10.6</v>
       </c>
       <c r="AK6" s="6">
-        <v>2.1600000000000001</v>
+        <v>2.16</v>
       </c>
       <c r="AL6" s="3">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AN6" s="5">
         <v>15.1</v>
       </c>
       <c r="AO6" s="5">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="AP6" s="3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AQ6" s="3">
         <v>2.113</v>
       </c>
       <c r="AR6" s="3">
-        <v>0.0060000000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AS6">
         <v>2</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>77</v>
+    <row r="7" spans="1:62">
+      <c r="A7" s="7">
+        <v>42170.5</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
@@ -1181,10 +1181,10 @@
         <v>67</v>
       </c>
       <c r="AB7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AC7" s="3">
-        <v>0.021999999999999999</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AD7" s="4">
         <v>1.1736</v>
@@ -1193,7 +1193,7 @@
         <v>8</v>
       </c>
       <c r="AF7" s="5">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="AG7">
         <v>114</v>
@@ -1208,16 +1208,16 @@
         <v>9.5</v>
       </c>
       <c r="AK7" s="5">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="AL7" s="3">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AN7" s="5">
-        <v>18.800000000000001</v>
+        <v>18.8</v>
       </c>
       <c r="AO7" s="5">
-        <v>10.300000000000001</v>
+        <v>10.3</v>
       </c>
       <c r="AP7">
         <v>0</v>
@@ -1226,15 +1226,15 @@
         <v>1.5389999999999999</v>
       </c>
       <c r="AR7" s="3">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AS7" s="5">
-        <v>2.7000000000000002</v>
+        <v>2.7</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>79</v>
+    <row r="8" spans="1:62">
+      <c r="A8" s="7">
+        <v>42200.5</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
@@ -1258,25 +1258,25 @@
         <v>67</v>
       </c>
       <c r="AB8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AC8" s="3">
-        <v>0.042999999999999997</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="AD8" s="6">
-        <v>0.93999999999999995</v>
+        <v>0.94</v>
       </c>
       <c r="AE8" s="5">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="AF8" s="5">
-        <v>2.6000000000000001</v>
+        <v>2.6</v>
       </c>
       <c r="AG8">
         <v>122</v>
       </c>
       <c r="AH8" s="5">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="AI8" s="5">
         <v>1.7</v>
@@ -1288,13 +1288,13 @@
         <v>1.3759999999999999</v>
       </c>
       <c r="AL8" s="3">
-        <v>0.0089999999999999993</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AN8" s="5">
-        <v>23.899999999999999</v>
+        <v>23.9</v>
       </c>
       <c r="AO8" s="5">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="AP8">
         <v>0</v>
@@ -1303,15 +1303,15 @@
         <v>1.349</v>
       </c>
       <c r="AR8" s="3">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AS8" s="5">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>81</v>
+    <row r="9" spans="1:62">
+      <c r="A9" s="7">
+        <v>42231.5</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
@@ -1335,16 +1335,16 @@
         <v>67</v>
       </c>
       <c r="AB9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="AC9" s="3">
-        <v>0.029000000000000001</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AD9" s="3">
         <v>1.7170000000000001</v>
       </c>
       <c r="AE9" s="5">
-        <v>7.7999999999999998</v>
+        <v>7.8</v>
       </c>
       <c r="AF9" s="5">
         <v>3.5</v>
@@ -1356,7 +1356,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AI9" s="5">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="AJ9" s="5">
         <v>8.1999999999999993</v>
@@ -1365,30 +1365,30 @@
         <v>2.2360000000000002</v>
       </c>
       <c r="AL9" s="3">
-        <v>0.017999999999999999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="AN9" s="5">
-        <v>23.600000000000001</v>
+        <v>23.6</v>
       </c>
       <c r="AO9" s="5">
-        <v>12.800000000000001</v>
+        <v>12.8</v>
       </c>
       <c r="AP9" s="3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AQ9" s="3">
         <v>2.2210000000000001</v>
       </c>
       <c r="AR9" s="3">
-        <v>0.010999999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="AS9" s="5">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>83</v>
+    <row r="10" spans="1:62">
+      <c r="A10" s="7">
+        <v>42262.5</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
@@ -1412,16 +1412,16 @@
         <v>67</v>
       </c>
       <c r="AB10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="AC10" s="3">
-        <v>0.0089999999999999993</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AD10" s="3">
         <v>1.4650000000000001</v>
       </c>
       <c r="AE10" s="5">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="AF10" s="5">
         <v>3.5</v>
@@ -1433,22 +1433,22 @@
         <v>1</v>
       </c>
       <c r="AI10" s="5">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="AJ10" s="5">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="AK10" s="3">
         <v>1.6679999999999999</v>
       </c>
       <c r="AL10" s="3">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AN10" s="5">
-        <v>24.399999999999999</v>
+        <v>24.4</v>
       </c>
       <c r="AO10" s="5">
-        <v>14.199999999999999</v>
+        <v>14.2</v>
       </c>
       <c r="AP10">
         <v>0</v>
@@ -1457,15 +1457,15 @@
         <v>1.6519999999999999</v>
       </c>
       <c r="AR10" s="3">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AS10" s="5">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:62">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
         <v>63</v>
@@ -1489,25 +1489,25 @@
         <v>67</v>
       </c>
       <c r="AB11" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="AC11" s="3">
-        <v>0.021000000000000001</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AD11" s="3">
         <v>1.119</v>
       </c>
       <c r="AE11" s="5">
-        <v>6.4000000000000004</v>
+        <v>6.4</v>
       </c>
       <c r="AF11" s="5">
-        <v>3.2999999999999998</v>
+        <v>3.3</v>
       </c>
       <c r="AG11">
         <v>119</v>
       </c>
       <c r="AH11" s="5">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="AI11" s="5">
         <v>2.5</v>
@@ -1519,30 +1519,30 @@
         <v>1.4870000000000001</v>
       </c>
       <c r="AL11" s="3">
-        <v>0.010999999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="AN11" s="5">
-        <v>20.699999999999999</v>
+        <v>20.7</v>
       </c>
       <c r="AO11">
         <v>9</v>
       </c>
       <c r="AP11" s="3">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AQ11" s="3">
         <v>1.4610000000000001</v>
       </c>
       <c r="AR11" s="3">
-        <v>0.0070000000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AS11" s="5">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>87</v>
+    <row r="12" spans="1:62">
+      <c r="A12" s="7">
+        <v>42323.5</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
@@ -1566,25 +1566,25 @@
         <v>67</v>
       </c>
       <c r="AB12" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AC12" s="3">
-        <v>0.044999999999999998</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AD12" s="3">
         <v>1.1850000000000001</v>
       </c>
       <c r="AE12" s="5">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="AF12" s="5">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="AG12">
         <v>122</v>
       </c>
       <c r="AH12" s="5">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="AI12" s="5">
         <v>2.2999999999999998</v>
@@ -1596,30 +1596,30 @@
         <v>1.4219999999999999</v>
       </c>
       <c r="AL12" s="3">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AN12" s="5">
         <v>14.6</v>
       </c>
       <c r="AO12" s="5">
-        <v>6.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="AP12" s="3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AQ12" s="3">
         <v>1.4059999999999999</v>
       </c>
       <c r="AR12" s="3">
-        <v>0.0070000000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AS12" s="5">
         <v>1.7</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>89</v>
+    <row r="13" spans="1:62">
+      <c r="A13" s="7">
+        <v>42353.5</v>
       </c>
       <c r="B13" t="s">
         <v>63</v>
@@ -1643,19 +1643,19 @@
         <v>67</v>
       </c>
       <c r="AB13" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AC13" s="3">
-        <v>0.032000000000000001</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="AD13" s="3">
         <v>1.7809999999999999</v>
       </c>
       <c r="AE13" s="5">
-        <v>7.7000000000000002</v>
+        <v>7.7</v>
       </c>
       <c r="AF13" s="5">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="AG13">
         <v>134</v>
@@ -1676,25 +1676,26 @@
         <v>0.01</v>
       </c>
       <c r="AN13" s="5">
-        <v>7.7000000000000002</v>
+        <v>7.7</v>
       </c>
       <c r="AO13" s="5">
-        <v>5.2999999999999998</v>
+        <v>5.3</v>
       </c>
       <c r="AP13" s="3">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AQ13" s="3">
         <v>1.8140000000000001</v>
       </c>
       <c r="AR13" s="3">
-        <v>0.0060000000000000001</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="AS13" s="5">
         <v>1.7</v>
       </c>
     </row>
-    <row r="14"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>